<commit_message>
Added command for rewrite is_luxury
</commit_message>
<xml_diff>
--- a/data_ocean/fixtures/luxury_cars_2017.xlsx
+++ b/data_ocean/fixtures/luxury_cars_2017.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2153" uniqueCount="512">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2153" uniqueCount="510">
   <si>
     <t xml:space="preserve">Перелік легкових автомобілів, з року випуску яким минуло не більше п’яти років (включно) та середньоринкова вартість яких становить понад 375  розмірів мінімальної заробітної  плати, встановленої законом на 1 січня 2017 (звітного) року</t>
   </si>
@@ -1523,19 +1523,13 @@
     <t xml:space="preserve">С63 Coupe </t>
   </si>
   <si>
-    <t xml:space="preserve">Mercedes-AMG C 63</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mercedes-AMG C 63 S</t>
+    <t xml:space="preserve">AMG C 63</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AMG C 63 S</t>
   </si>
   <si>
     <t xml:space="preserve">С63 Sedan </t>
-  </si>
-  <si>
-    <t xml:space="preserve">AMG C 63</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AMG C 63 S</t>
   </si>
   <si>
     <t xml:space="preserve">E-Class Cabrio</t>
@@ -2287,8 +2281,8 @@
   </sheetPr>
   <dimension ref="A1:N628"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="B67" colorId="64" zoomScale="110" zoomScaleNormal="100" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C117" activeCellId="0" sqref="C117"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A572" colorId="64" zoomScale="110" zoomScaleNormal="100" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B429" activeCellId="0" sqref="B429"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.96484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9415,7 +9409,7 @@
         <v>299</v>
       </c>
       <c r="B431" s="11" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="C431" s="6" t="s">
         <v>9</v>
@@ -9429,7 +9423,7 @@
         <v>299</v>
       </c>
       <c r="B432" s="11" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="C432" s="6" t="s">
         <v>9</v>
@@ -9443,7 +9437,7 @@
         <v>299</v>
       </c>
       <c r="B433" s="5" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="C433" s="6" t="s">
         <v>9</v>
@@ -9461,7 +9455,7 @@
         <v>299</v>
       </c>
       <c r="B434" s="11" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="C434" s="6" t="s">
         <v>9</v>
@@ -9475,7 +9469,7 @@
         <v>299</v>
       </c>
       <c r="B435" s="5" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="C435" s="6" t="s">
         <v>9</v>
@@ -9493,7 +9487,7 @@
         <v>299</v>
       </c>
       <c r="B436" s="5" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C436" s="6" t="s">
         <v>9</v>
@@ -9511,7 +9505,7 @@
         <v>299</v>
       </c>
       <c r="B437" s="11" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="C437" s="6" t="s">
         <v>9</v>
@@ -9525,7 +9519,7 @@
         <v>299</v>
       </c>
       <c r="B438" s="11" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="C438" s="6" t="s">
         <v>9</v>
@@ -9539,7 +9533,7 @@
         <v>299</v>
       </c>
       <c r="B439" s="5" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="C439" s="6" t="s">
         <v>9</v>
@@ -9557,7 +9551,7 @@
         <v>299</v>
       </c>
       <c r="B440" s="11" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C440" s="6" t="s">
         <v>9</v>
@@ -9571,7 +9565,7 @@
         <v>299</v>
       </c>
       <c r="B441" s="5" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C441" s="6" t="s">
         <v>9</v>
@@ -9589,7 +9583,7 @@
         <v>299</v>
       </c>
       <c r="B442" s="11" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="C442" s="6" t="s">
         <v>9</v>
@@ -9603,7 +9597,7 @@
         <v>299</v>
       </c>
       <c r="B443" s="11" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="C443" s="25" t="s">
         <v>9</v>
@@ -9635,7 +9629,7 @@
         <v>299</v>
       </c>
       <c r="B445" s="11" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="C445" s="6" t="s">
         <v>9</v>
@@ -9649,7 +9643,7 @@
         <v>299</v>
       </c>
       <c r="B446" s="11" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="C446" s="6" t="s">
         <v>9</v>
@@ -9663,7 +9657,7 @@
         <v>299</v>
       </c>
       <c r="B447" s="5" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="C447" s="6" t="s">
         <v>9</v>
@@ -9681,7 +9675,7 @@
         <v>299</v>
       </c>
       <c r="B448" s="5" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="C448" s="6" t="s">
         <v>9</v>
@@ -9713,7 +9707,7 @@
         <v>299</v>
       </c>
       <c r="B450" s="11" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="C450" s="6" t="s">
         <v>9</v>
@@ -9727,7 +9721,7 @@
         <v>299</v>
       </c>
       <c r="B451" s="11" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C451" s="6" t="s">
         <v>9</v>
@@ -9741,7 +9735,7 @@
         <v>299</v>
       </c>
       <c r="B452" s="5" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C452" s="6" t="s">
         <v>9</v>
@@ -9759,7 +9753,7 @@
         <v>299</v>
       </c>
       <c r="B453" s="11" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="C453" s="6" t="s">
         <v>9</v>
@@ -9773,7 +9767,7 @@
         <v>299</v>
       </c>
       <c r="B454" s="11" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="C454" s="6" t="s">
         <v>9</v>
@@ -9805,7 +9799,7 @@
         <v>299</v>
       </c>
       <c r="B456" s="11" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="C456" s="6" t="s">
         <v>9</v>
@@ -9819,7 +9813,7 @@
         <v>299</v>
       </c>
       <c r="B457" s="11" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="C457" s="6" t="s">
         <v>9</v>
@@ -9833,7 +9827,7 @@
         <v>299</v>
       </c>
       <c r="B458" s="5" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="C458" s="6" t="s">
         <v>9</v>
@@ -9851,7 +9845,7 @@
         <v>299</v>
       </c>
       <c r="B459" s="11" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C459" s="6" t="s">
         <v>9</v>
@@ -9883,7 +9877,7 @@
         <v>299</v>
       </c>
       <c r="B461" s="11" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="C461" s="6" t="s">
         <v>9</v>
@@ -9915,7 +9909,7 @@
         <v>299</v>
       </c>
       <c r="B463" s="11" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="C463" s="6" t="s">
         <v>9</v>
@@ -9929,7 +9923,7 @@
         <v>299</v>
       </c>
       <c r="B464" s="11" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="C464" s="6" t="s">
         <v>9</v>
@@ -9961,7 +9955,7 @@
         <v>299</v>
       </c>
       <c r="B466" s="11" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="C466" s="6" t="s">
         <v>9</v>
@@ -9975,7 +9969,7 @@
         <v>299</v>
       </c>
       <c r="B467" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C467" s="6" t="s">
         <v>9</v>
@@ -9989,7 +9983,7 @@
         <v>299</v>
       </c>
       <c r="B468" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="C468" s="6" t="s">
         <v>9</v>
@@ -10003,7 +9997,7 @@
         <v>299</v>
       </c>
       <c r="B469" s="5" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="C469" s="6" t="s">
         <v>12</v>
@@ -10021,7 +10015,7 @@
         <v>299</v>
       </c>
       <c r="B470" s="11" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="C470" s="6" t="s">
         <v>12</v>
@@ -10035,7 +10029,7 @@
         <v>299</v>
       </c>
       <c r="B471" s="5" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="C471" s="6" t="s">
         <v>12</v>
@@ -10053,7 +10047,7 @@
         <v>299</v>
       </c>
       <c r="B472" s="11" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="C472" s="6" t="s">
         <v>12</v>
@@ -10085,7 +10079,7 @@
         <v>299</v>
       </c>
       <c r="B474" s="11" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C474" s="6" t="s">
         <v>12</v>
@@ -10099,7 +10093,7 @@
         <v>299</v>
       </c>
       <c r="B475" s="11" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="C475" s="6" t="s">
         <v>12</v>
@@ -10113,7 +10107,7 @@
         <v>299</v>
       </c>
       <c r="B476" s="5" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="C476" s="6" t="s">
         <v>12</v>
@@ -10131,7 +10125,7 @@
         <v>299</v>
       </c>
       <c r="B477" s="11" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C477" s="6" t="s">
         <v>12</v>
@@ -10145,7 +10139,7 @@
         <v>299</v>
       </c>
       <c r="B478" s="5" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="C478" s="6" t="s">
         <v>12</v>
@@ -10163,7 +10157,7 @@
         <v>299</v>
       </c>
       <c r="B479" s="11" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C479" s="6" t="s">
         <v>12</v>
@@ -10177,7 +10171,7 @@
         <v>299</v>
       </c>
       <c r="B480" s="5" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="C480" s="6" t="s">
         <v>12</v>
@@ -10195,7 +10189,7 @@
         <v>299</v>
       </c>
       <c r="B481" s="11" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C481" s="6" t="s">
         <v>12</v>
@@ -10227,7 +10221,7 @@
         <v>299</v>
       </c>
       <c r="B483" s="11" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C483" s="6" t="s">
         <v>12</v>
@@ -10241,7 +10235,7 @@
         <v>299</v>
       </c>
       <c r="B484" s="11" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="C484" s="6" t="s">
         <v>12</v>
@@ -10255,7 +10249,7 @@
         <v>299</v>
       </c>
       <c r="B485" s="5" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="C485" s="6" t="s">
         <v>12</v>
@@ -10273,7 +10267,7 @@
         <v>299</v>
       </c>
       <c r="B486" s="5" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="C486" s="6" t="s">
         <v>12</v>
@@ -10291,7 +10285,7 @@
         <v>299</v>
       </c>
       <c r="B487" s="11" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C487" s="6" t="s">
         <v>12</v>
@@ -10305,7 +10299,7 @@
         <v>299</v>
       </c>
       <c r="B488" s="5" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C488" s="6" t="s">
         <v>12</v>
@@ -10323,7 +10317,7 @@
         <v>299</v>
       </c>
       <c r="B489" s="11" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C489" s="6" t="s">
         <v>12</v>
@@ -10337,7 +10331,7 @@
         <v>299</v>
       </c>
       <c r="B490" s="11" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C490" s="6" t="s">
         <v>12</v>
@@ -10351,7 +10345,7 @@
         <v>299</v>
       </c>
       <c r="B491" s="11" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="C491" s="6" t="s">
         <v>12</v>
@@ -10365,7 +10359,7 @@
         <v>299</v>
       </c>
       <c r="B492" s="5" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C492" s="6" t="s">
         <v>12</v>
@@ -10383,7 +10377,7 @@
         <v>299</v>
       </c>
       <c r="B493" s="11" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="C493" s="6" t="s">
         <v>12</v>
@@ -10397,7 +10391,7 @@
         <v>299</v>
       </c>
       <c r="B494" s="11" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="C494" s="6" t="s">
         <v>12</v>
@@ -10411,7 +10405,7 @@
         <v>299</v>
       </c>
       <c r="B495" s="11" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="C495" s="6" t="s">
         <v>12</v>
@@ -10425,7 +10419,7 @@
         <v>299</v>
       </c>
       <c r="B496" s="5" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="C496" s="6" t="s">
         <v>12</v>
@@ -10443,7 +10437,7 @@
         <v>299</v>
       </c>
       <c r="B497" s="11" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C497" s="6" t="s">
         <v>12</v>
@@ -10457,7 +10451,7 @@
         <v>299</v>
       </c>
       <c r="B498" s="5" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="C498" s="6" t="s">
         <v>12</v>
@@ -10475,7 +10469,7 @@
         <v>299</v>
       </c>
       <c r="B499" s="11" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="C499" s="25" t="s">
         <v>12</v>
@@ -10489,7 +10483,7 @@
         <v>299</v>
       </c>
       <c r="B500" s="5" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="C500" s="6" t="s">
         <v>12</v>
@@ -10507,7 +10501,7 @@
         <v>299</v>
       </c>
       <c r="B501" s="11" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="C501" s="6" t="s">
         <v>12</v>
@@ -10521,7 +10515,7 @@
         <v>299</v>
       </c>
       <c r="B502" s="5" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="C502" s="6" t="s">
         <v>12</v>
@@ -10539,7 +10533,7 @@
         <v>299</v>
       </c>
       <c r="B503" s="11" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="C503" s="6" t="s">
         <v>12</v>
@@ -10553,7 +10547,7 @@
         <v>299</v>
       </c>
       <c r="B504" s="5" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="C504" s="6" t="s">
         <v>12</v>
@@ -10571,7 +10565,7 @@
         <v>299</v>
       </c>
       <c r="B505" s="11" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C505" s="6" t="s">
         <v>12</v>
@@ -10585,7 +10579,7 @@
         <v>299</v>
       </c>
       <c r="B506" s="11" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="C506" s="6" t="s">
         <v>12</v>
@@ -10599,7 +10593,7 @@
         <v>299</v>
       </c>
       <c r="B507" s="11" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="C507" s="6" t="s">
         <v>12</v>
@@ -10613,7 +10607,7 @@
         <v>299</v>
       </c>
       <c r="B508" s="5" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="C508" s="6" t="s">
         <v>12</v>
@@ -10631,7 +10625,7 @@
         <v>299</v>
       </c>
       <c r="B509" s="11" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="C509" s="6" t="s">
         <v>12</v>
@@ -10645,7 +10639,7 @@
         <v>299</v>
       </c>
       <c r="B510" s="5" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="C510" s="6" t="s">
         <v>12</v>
@@ -10663,7 +10657,7 @@
         <v>299</v>
       </c>
       <c r="B511" s="11" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="C511" s="6" t="s">
         <v>12</v>
@@ -10677,7 +10671,7 @@
         <v>299</v>
       </c>
       <c r="B512" s="11" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="C512" s="6" t="s">
         <v>12</v>
@@ -10691,7 +10685,7 @@
         <v>299</v>
       </c>
       <c r="B513" s="5" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C513" s="6" t="s">
         <v>12</v>
@@ -10709,7 +10703,7 @@
         <v>299</v>
       </c>
       <c r="B514" s="11" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="C514" s="6" t="s">
         <v>12</v>
@@ -10723,7 +10717,7 @@
         <v>299</v>
       </c>
       <c r="B515" s="11" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="C515" s="6" t="s">
         <v>12</v>
@@ -10737,7 +10731,7 @@
         <v>299</v>
       </c>
       <c r="B516" s="11" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="C516" s="6" t="s">
         <v>12</v>
@@ -10751,7 +10745,7 @@
         <v>299</v>
       </c>
       <c r="B517" s="5" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="C517" s="6" t="s">
         <v>12</v>
@@ -10769,7 +10763,7 @@
         <v>299</v>
       </c>
       <c r="B518" s="8" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C518" s="6"/>
       <c r="D518" s="7"/>
@@ -10781,7 +10775,7 @@
         <v>299</v>
       </c>
       <c r="B519" s="5" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="C519" s="6" t="s">
         <v>12</v>
@@ -10799,7 +10793,7 @@
         <v>299</v>
       </c>
       <c r="B520" s="11" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="C520" s="6" t="s">
         <v>12</v>
@@ -10813,7 +10807,7 @@
         <v>299</v>
       </c>
       <c r="B521" s="5" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="C521" s="6" t="s">
         <v>12</v>
@@ -10831,7 +10825,7 @@
         <v>299</v>
       </c>
       <c r="B522" s="11" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="C522" s="6" t="s">
         <v>12</v>
@@ -10845,7 +10839,7 @@
         <v>299</v>
       </c>
       <c r="B523" s="11" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="C523" s="6" t="s">
         <v>12</v>
@@ -10877,7 +10871,7 @@
         <v>299</v>
       </c>
       <c r="B525" s="31" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="C525" s="6" t="s">
         <v>15</v>
@@ -10888,10 +10882,10 @@
     </row>
     <row r="526" s="9" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A526" s="5" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="B526" s="5" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="C526" s="6" t="s">
         <v>15</v>
@@ -10906,10 +10900,10 @@
     </row>
     <row r="527" s="9" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A527" s="5" t="s">
+        <v>456</v>
+      </c>
+      <c r="B527" s="5" t="s">
         <v>458</v>
-      </c>
-      <c r="B527" s="5" t="s">
-        <v>460</v>
       </c>
       <c r="C527" s="6" t="s">
         <v>9</v>
@@ -10924,10 +10918,10 @@
     </row>
     <row r="528" s="9" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A528" s="5" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="B528" s="5" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="C528" s="6" t="s">
         <v>9</v>
@@ -10942,10 +10936,10 @@
     </row>
     <row r="529" s="9" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A529" s="5" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="B529" s="5" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="C529" s="6" t="s">
         <v>12</v>
@@ -10960,7 +10954,7 @@
     </row>
     <row r="530" s="9" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A530" s="5" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="B530" s="5" t="n">
         <v>918</v>
@@ -10978,10 +10972,10 @@
     </row>
     <row r="531" s="9" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A531" s="5" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="B531" s="5" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="C531" s="6" t="s">
         <v>15</v>
@@ -10998,10 +10992,10 @@
     </row>
     <row r="532" s="9" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A532" s="5" t="s">
+        <v>461</v>
+      </c>
+      <c r="B532" s="5" t="s">
         <v>463</v>
-      </c>
-      <c r="B532" s="5" t="s">
-        <v>465</v>
       </c>
       <c r="C532" s="6" t="s">
         <v>15</v>
@@ -11018,10 +11012,10 @@
     </row>
     <row r="533" s="9" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A533" s="5" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="B533" s="5" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="C533" s="6" t="s">
         <v>15</v>
@@ -11038,10 +11032,10 @@
     </row>
     <row r="534" s="9" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A534" s="5" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="B534" s="5" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="C534" s="6" t="s">
         <v>15</v>
@@ -11058,10 +11052,10 @@
     </row>
     <row r="535" s="9" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A535" s="5" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="B535" s="5" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="C535" s="6" t="s">
         <v>15</v>
@@ -11076,10 +11070,10 @@
     </row>
     <row r="536" s="9" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A536" s="5" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="B536" s="5" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="C536" s="6" t="s">
         <v>15</v>
@@ -11096,10 +11090,10 @@
     </row>
     <row r="537" s="9" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A537" s="5" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="B537" s="5" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="C537" s="6" t="s">
         <v>15</v>
@@ -11116,10 +11110,10 @@
     </row>
     <row r="538" s="9" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A538" s="5" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="B538" s="5" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="C538" s="6" t="s">
         <v>15</v>
@@ -11136,10 +11130,10 @@
     </row>
     <row r="539" s="9" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A539" s="5" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="B539" s="5" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="C539" s="6" t="s">
         <v>15</v>
@@ -11154,10 +11148,10 @@
     </row>
     <row r="540" s="9" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A540" s="12" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="B540" s="13" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="C540" s="32" t="s">
         <v>39</v>
@@ -11172,10 +11166,10 @@
     </row>
     <row r="541" s="9" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A541" s="5" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="B541" s="5" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="C541" s="6" t="s">
         <v>15</v>
@@ -11190,10 +11184,10 @@
     </row>
     <row r="542" s="9" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A542" s="5" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="B542" s="5" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="C542" s="6" t="s">
         <v>48</v>
@@ -11208,10 +11202,10 @@
     </row>
     <row r="543" s="9" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A543" s="5" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="B543" s="5" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="C543" s="6" t="s">
         <v>48</v>
@@ -11226,10 +11220,10 @@
     </row>
     <row r="544" s="9" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A544" s="5" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="B544" s="5" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="C544" s="6" t="s">
         <v>9</v>
@@ -11244,10 +11238,10 @@
     </row>
     <row r="545" s="9" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A545" s="5" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="B545" s="5" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="C545" s="6" t="s">
         <v>9</v>
@@ -11262,10 +11256,10 @@
     </row>
     <row r="546" s="9" customFormat="true" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A546" s="5" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="B546" s="5" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="C546" s="6" t="s">
         <v>9</v>
@@ -11280,10 +11274,10 @@
     </row>
     <row r="547" s="9" customFormat="true" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A547" s="5" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="B547" s="11" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="C547" s="6" t="s">
         <v>9</v>
@@ -11294,10 +11288,10 @@
     </row>
     <row r="548" s="9" customFormat="true" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A548" s="5" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="B548" s="11" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="C548" s="6" t="s">
         <v>9</v>
@@ -11308,10 +11302,10 @@
     </row>
     <row r="549" s="9" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A549" s="5" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="B549" s="5" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="C549" s="6" t="s">
         <v>9</v>
@@ -11326,10 +11320,10 @@
     </row>
     <row r="550" s="9" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A550" s="5" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="B550" s="5" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="C550" s="6" t="s">
         <v>9</v>
@@ -11346,10 +11340,10 @@
     </row>
     <row r="551" s="9" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A551" s="5" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="B551" s="5" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="C551" s="6" t="s">
         <v>9</v>
@@ -11364,10 +11358,10 @@
     </row>
     <row r="552" s="9" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A552" s="5" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="B552" s="5" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="C552" s="6" t="s">
         <v>12</v>
@@ -11382,10 +11376,10 @@
     </row>
     <row r="553" s="9" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A553" s="5" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="B553" s="11" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="C553" s="6" t="s">
         <v>12</v>
@@ -11396,10 +11390,10 @@
     </row>
     <row r="554" s="9" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A554" s="5" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="B554" s="11" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="C554" s="6" t="s">
         <v>12</v>
@@ -11410,10 +11404,10 @@
     </row>
     <row r="555" s="9" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A555" s="5" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="B555" s="5" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="C555" s="6" t="s">
         <v>12</v>
@@ -11428,10 +11422,10 @@
     </row>
     <row r="556" s="33" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A556" s="5" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="B556" s="5" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="C556" s="6" t="s">
         <v>12</v>
@@ -11448,10 +11442,10 @@
     </row>
     <row r="557" s="33" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A557" s="5" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="B557" s="5" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="C557" s="6" t="s">
         <v>12</v>
@@ -11466,10 +11460,10 @@
     </row>
     <row r="558" s="9" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A558" s="5" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="B558" s="5" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="C558" s="6" t="s">
         <v>15</v>
@@ -11484,10 +11478,10 @@
     </row>
     <row r="559" s="9" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A559" s="5" t="s">
+        <v>477</v>
+      </c>
+      <c r="B559" s="5" t="s">
         <v>479</v>
-      </c>
-      <c r="B559" s="5" t="s">
-        <v>481</v>
       </c>
       <c r="C559" s="6" t="s">
         <v>15</v>
@@ -11502,10 +11496,10 @@
     </row>
     <row r="560" s="9" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A560" s="5" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="B560" s="5" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="C560" s="6" t="s">
         <v>15</v>
@@ -11520,10 +11514,10 @@
     </row>
     <row r="561" s="9" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A561" s="5" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="B561" s="5" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="C561" s="6" t="s">
         <v>15</v>
@@ -11538,10 +11532,10 @@
     </row>
     <row r="562" s="9" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A562" s="5" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="B562" s="5" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="C562" s="6" t="s">
         <v>39</v>
@@ -11556,10 +11550,10 @@
     </row>
     <row r="563" s="9" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A563" s="5" t="s">
+        <v>482</v>
+      </c>
+      <c r="B563" s="5" t="s">
         <v>484</v>
-      </c>
-      <c r="B563" s="5" t="s">
-        <v>486</v>
       </c>
       <c r="C563" s="6" t="s">
         <v>39</v>
@@ -11574,10 +11568,10 @@
     </row>
     <row r="564" s="9" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A564" s="5" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="B564" s="5" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="C564" s="6" t="s">
         <v>9</v>
@@ -11592,10 +11586,10 @@
     </row>
     <row r="565" s="9" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A565" s="5" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="B565" s="5" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="C565" s="6" t="s">
         <v>9</v>
@@ -11610,10 +11604,10 @@
     </row>
     <row r="566" s="9" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A566" s="5" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="B566" s="5" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="C566" s="6" t="s">
         <v>12</v>
@@ -11628,10 +11622,10 @@
     </row>
     <row r="567" s="9" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A567" s="5" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="B567" s="5" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="C567" s="6" t="s">
         <v>12</v>
@@ -11646,10 +11640,10 @@
     </row>
     <row r="568" s="9" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A568" s="5" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="B568" s="5" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="C568" s="6" t="s">
         <v>12</v>
@@ -11664,10 +11658,10 @@
     </row>
     <row r="569" s="9" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A569" s="5" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="B569" s="5" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="C569" s="6" t="s">
         <v>12</v>
@@ -11682,10 +11676,10 @@
     </row>
     <row r="570" s="9" customFormat="true" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A570" s="5" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="B570" s="5" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="C570" s="6" t="s">
         <v>12</v>
@@ -11700,10 +11694,10 @@
     </row>
     <row r="571" s="9" customFormat="true" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A571" s="5" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="B571" s="11" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="C571" s="6" t="s">
         <v>12</v>
@@ -11714,10 +11708,10 @@
     </row>
     <row r="572" s="9" customFormat="true" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A572" s="5" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="B572" s="11" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="C572" s="6" t="s">
         <v>12</v>
@@ -11728,10 +11722,10 @@
     </row>
     <row r="573" s="9" customFormat="true" ht="33.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A573" s="5" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="B573" s="5" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="C573" s="6" t="s">
         <v>12</v>
@@ -11746,10 +11740,10 @@
     </row>
     <row r="574" s="9" customFormat="true" ht="33.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A574" s="5" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="B574" s="11" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="C574" s="6" t="s">
         <v>12</v>
@@ -11760,10 +11754,10 @@
     </row>
     <row r="575" s="9" customFormat="true" ht="33.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A575" s="5" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="B575" s="11" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="C575" s="6" t="s">
         <v>12</v>
@@ -11774,10 +11768,10 @@
     </row>
     <row r="576" s="9" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A576" s="5" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="B576" s="5" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="C576" s="6" t="s">
         <v>12</v>
@@ -11792,10 +11786,10 @@
     </row>
     <row r="577" s="9" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A577" s="5" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="B577" s="5" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="C577" s="6" t="s">
         <v>15</v>
@@ -11810,10 +11804,10 @@
     </row>
     <row r="578" s="9" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A578" s="5" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="B578" s="5" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="C578" s="6" t="s">
         <v>9</v>
@@ -11828,10 +11822,10 @@
     </row>
     <row r="579" s="9" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A579" s="5" t="s">
+        <v>495</v>
+      </c>
+      <c r="B579" s="5" t="s">
         <v>497</v>
-      </c>
-      <c r="B579" s="5" t="s">
-        <v>499</v>
       </c>
       <c r="C579" s="6" t="s">
         <v>12</v>
@@ -11846,10 +11840,10 @@
     </row>
     <row r="580" s="9" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A580" s="5" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="B580" s="5" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="C580" s="6" t="s">
         <v>12</v>
@@ -11864,10 +11858,10 @@
     </row>
     <row r="581" s="9" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A581" s="5" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="B581" s="5" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="C581" s="6" t="s">
         <v>12</v>
@@ -11882,10 +11876,10 @@
     </row>
     <row r="582" s="9" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A582" s="5" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="B582" s="5" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="C582" s="6" t="s">
         <v>12</v>
@@ -11900,10 +11894,10 @@
     </row>
     <row r="583" s="9" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A583" s="5" t="s">
+        <v>495</v>
+      </c>
+      <c r="B583" s="5" t="s">
         <v>497</v>
-      </c>
-      <c r="B583" s="5" t="s">
-        <v>499</v>
       </c>
       <c r="C583" s="6" t="s">
         <v>12</v>
@@ -11918,10 +11912,10 @@
     </row>
     <row r="584" s="9" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A584" s="5" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B584" s="5" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="C584" s="6" t="s">
         <v>12</v>
@@ -11936,10 +11930,10 @@
     </row>
     <row r="585" s="9" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A585" s="5" t="s">
+        <v>500</v>
+      </c>
+      <c r="B585" s="5" t="s">
         <v>502</v>
-      </c>
-      <c r="B585" s="5" t="s">
-        <v>504</v>
       </c>
       <c r="C585" s="6" t="s">
         <v>12</v>
@@ -11954,10 +11948,10 @@
     </row>
     <row r="586" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A586" s="12" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="B586" s="13" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="C586" s="6" t="s">
         <v>9</v>
@@ -11968,10 +11962,10 @@
     </row>
     <row r="587" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A587" s="12" t="s">
+        <v>503</v>
+      </c>
+      <c r="B587" s="13" t="s">
         <v>505</v>
-      </c>
-      <c r="B587" s="13" t="s">
-        <v>507</v>
       </c>
       <c r="C587" s="6" t="s">
         <v>39</v>
@@ -11982,10 +11976,10 @@
     </row>
     <row r="588" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A588" s="12" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="B588" s="13" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="C588" s="6" t="s">
         <v>15</v>
@@ -11996,10 +11990,10 @@
     </row>
     <row r="589" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A589" s="12" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="B589" s="13" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="C589" s="6" t="s">
         <v>9</v>
@@ -12010,10 +12004,10 @@
     </row>
     <row r="590" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A590" s="12" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="B590" s="13" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="C590" s="6" t="s">
         <v>39</v>
@@ -12024,10 +12018,10 @@
     </row>
     <row r="591" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A591" s="12" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="B591" s="13" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="C591" s="6" t="s">
         <v>15</v>

</xml_diff>